<commit_message>
Looping with forEach - Building HTML Tables
</commit_message>
<xml_diff>
--- a/me_docs/5.JSP-Standard-Tag-Library-Core-Tags.xlsx
+++ b/me_docs/5.JSP-Standard-Tag-Library-Core-Tags.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4077D33E-A620-466F-908D-A5293C1CA689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60227B2-2BD1-4ADD-94E4-412F671F5B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create project" sheetId="1" r:id="rId1"/>
     <sheet name="download jar" sheetId="2" r:id="rId2"/>
     <sheet name="test jsp" sheetId="3" r:id="rId3"/>
     <sheet name="foreach-simple" sheetId="4" r:id="rId4"/>
+    <sheet name="foreach-student" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Create Dynamic Web Project</t>
   </si>
@@ -67,6 +68,24 @@
   </si>
   <si>
     <t>Access URL to test: http://localhost:8080/tagdemo/foreach-simple-test.jsp</t>
+  </si>
+  <si>
+    <t>Create tagdemo package</t>
+  </si>
+  <si>
+    <t>Create Student Class</t>
+  </si>
+  <si>
+    <t>Create Constructor using Fields</t>
+  </si>
+  <si>
+    <t>Generate Getters and Setters</t>
+  </si>
+  <si>
+    <t>Create foreach-student-test.jsp</t>
+  </si>
+  <si>
+    <t>Access URL to test: http://localhost:8080/tagdemo/foreach-student-test.jsp</t>
   </si>
 </sst>
 </file>
@@ -966,6 +985,715 @@
         <a:xfrm>
           <a:off x="609600" y="16192500"/>
           <a:ext cx="4923809" cy="1685714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180190</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>189881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B201CA7-BE63-45C9-853D-EF81A3DE3302}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="952500"/>
+          <a:ext cx="6276190" cy="4952381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>503543</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>28000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30F7E135-B761-4665-9067-A201F3249D10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="26479500"/>
+          <a:ext cx="10257143" cy="4600000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>466133</xdr:colOff>
+      <xdr:row>197</xdr:row>
+      <xdr:rowOff>84929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D08D331-1F15-4FD1-BB7C-8DBDBEDB5514}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="31242000"/>
+          <a:ext cx="4733333" cy="6371429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>179886</xdr:colOff>
+      <xdr:row>222</xdr:row>
+      <xdr:rowOff>37524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64064CC2-23A7-4798-9E56-57B53D6D886E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="37719000"/>
+          <a:ext cx="8714286" cy="4609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>225</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>446400</xdr:colOff>
+      <xdr:row>249</xdr:row>
+      <xdr:rowOff>37524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{646996B1-ECD3-4665-9277-86BE05D72350}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="42862500"/>
+          <a:ext cx="10200000" cy="4609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>570895</xdr:colOff>
+      <xdr:row>284</xdr:row>
+      <xdr:rowOff>65857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6811DE0-82F3-44D8-A4CD-46717DDE6064}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="47625000"/>
+          <a:ext cx="4838095" cy="6542857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>285</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>551848</xdr:colOff>
+      <xdr:row>319</xdr:row>
+      <xdr:rowOff>75381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05977CE6-DB77-493B-8A50-D1073B5824CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="54292500"/>
+          <a:ext cx="4819048" cy="6552381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>353</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>141790</xdr:colOff>
+      <xdr:row>377</xdr:row>
+      <xdr:rowOff>170857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A058D039-07C0-476D-9F1B-BC54E1C02F3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="61341000"/>
+          <a:ext cx="8676190" cy="4742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>379</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8914</xdr:colOff>
+      <xdr:row>408</xdr:row>
+      <xdr:rowOff>180262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FCB47BC-E072-4D70-82C2-581106E00796}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="66294000"/>
+          <a:ext cx="4885714" cy="5704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>18438</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>75690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE640840-2D07-46DA-800A-E43DFE2A2368}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5524500"/>
+          <a:ext cx="4895238" cy="4076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>189562</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>180357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0868CF8-14BF-4409-9998-A3A3AC477252}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="9906000"/>
+          <a:ext cx="7504762" cy="4942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>132724</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>104024</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{864A3F10-82D5-4BD5-BA8F-A65B8364ADBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="15049500"/>
+          <a:ext cx="5009524" cy="6009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>199314</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>66071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9379D42D-AAA8-4DBA-884D-7A2F2465984D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="21336000"/>
+          <a:ext cx="5685714" cy="4828571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>320</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>198933</xdr:colOff>
+      <xdr:row>350</xdr:row>
+      <xdr:rowOff>94524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F564CD65-5972-41F4-9C98-8D5DA58330E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="60960000"/>
+          <a:ext cx="8733333" cy="5809524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>410</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>237105</xdr:colOff>
+      <xdr:row>441</xdr:row>
+      <xdr:rowOff>104024</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E050E62-4FA5-40A7-A3B0-5811AA8927A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="78105000"/>
+          <a:ext cx="8161905" cy="6009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>444</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>18438</xdr:colOff>
+      <xdr:row>456</xdr:row>
+      <xdr:rowOff>94952</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{528C46D9-A1D7-491C-B85A-BBEB2F46E2F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="84582000"/>
+          <a:ext cx="4895238" cy="2380952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1345,7 +2073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA8A14A-8856-49AD-A710-A33247DA707E}">
   <dimension ref="A2:A85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="L95" sqref="L95"/>
     </sheetView>
   </sheetViews>
@@ -1365,4 +2093,50 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A92F222-D56F-4605-8ECA-E0D0CDC2877F}">
+  <dimension ref="A2:A444"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A448" workbookViewId="0">
+      <selection activeCell="N453" sqref="N453"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Testing Conditionals with the IF tag
</commit_message>
<xml_diff>
--- a/me_docs/5.JSP-Standard-Tag-Library-Core-Tags.xlsx
+++ b/me_docs/5.JSP-Standard-Tag-Library-Core-Tags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\JSP-Servlets-JDBC\me_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60227B2-2BD1-4ADD-94E4-412F671F5B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1165CE8-5F16-492F-AA51-EEC8FE50F1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create project" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="test jsp" sheetId="3" r:id="rId3"/>
     <sheet name="foreach-simple" sheetId="4" r:id="rId4"/>
     <sheet name="foreach-student" sheetId="5" r:id="rId5"/>
+    <sheet name="Conditionals" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Create Dynamic Web Project</t>
   </si>
@@ -87,6 +88,12 @@
   <si>
     <t>Access URL to test: http://localhost:8080/tagdemo/foreach-student-test.jsp</t>
   </si>
+  <si>
+    <t>Create if-student-test.jsp</t>
+  </si>
+  <si>
+    <t>Access URL to test: http://localhost:8080/tagdemo/if-student-test.jsp</t>
+  </si>
 </sst>
 </file>
 
@@ -1694,6 +1701,187 @@
         <a:xfrm>
           <a:off x="609600" y="84582000"/>
           <a:ext cx="4895238" cy="2380952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>141790</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>170857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CBD1CBF-1B30-430F-AAB0-1C1BA5E50AE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="8676190" cy="4742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>608990</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>189786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F9860CA-F637-45E6-BAF7-AA57C135B8B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5334000"/>
+          <a:ext cx="4876190" cy="5714286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>284800</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>37357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0B3683F-7067-4A25-B84D-AC2CE4A632C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="11239500"/>
+          <a:ext cx="7600000" cy="5942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>37486</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>18810</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39F84EF2-B4DF-4425-B9CD-60CFA11F2178}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="17716500"/>
+          <a:ext cx="4914286" cy="1923810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2099,8 +2287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A92F222-D56F-4605-8ECA-E0D0CDC2877F}">
   <dimension ref="A2:A444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A448" workbookViewId="0">
-      <selection activeCell="N453" sqref="N453"/>
+    <sheetView topLeftCell="A433" workbookViewId="0">
+      <selection activeCell="A444" sqref="A444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2139,4 +2327,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B524C3-D3F0-4C35-8308-C8DB7DA1A31D}">
+  <dimension ref="A2:A93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="P102" sqref="P102"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>